<commit_message>
Zakat & Tax SignUp Developed.
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager.xlsx
+++ b/src/test/resources/Run_Manager.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="96">
   <si>
     <t>P_Key</t>
   </si>
@@ -266,19 +266,49 @@
     <t>Sign up in Zakat And Tax Portal as Consortium Company.</t>
   </si>
   <si>
+    <t>AccountType</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>OtherAccountCategory</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Consortium</t>
+  </si>
+  <si>
+    <t>Company_ID</t>
+  </si>
+  <si>
+    <t>Company_Name</t>
+  </si>
+  <si>
+    <t>Contract_Number</t>
+  </si>
+  <si>
+    <t>Mobile_Number</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Confirm_Email</t>
+  </si>
+  <si>
+    <t>TestCrewConsortium</t>
+  </si>
+  <si>
+    <t>TestCrewConsortium@lab.testcrew.com</t>
+  </si>
+  <si>
+    <t>71234567890</t>
+  </si>
+  <si>
     <t>Passed</t>
-  </si>
-  <si>
-    <t>AccountType</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>OtherAccountCategory</t>
-  </si>
-  <si>
-    <t>Failed</t>
   </si>
 </sst>
 </file>
@@ -494,7 +524,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -553,6 +583,7 @@
     <xf numFmtId="49" fontId="2" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1459,7 +1490,7 @@
         <v>74</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="I3" s="27"/>
     </row>
@@ -1493,10 +1524,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1506,9 +1537,14 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="28.28515625" collapsed="false"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="false"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="21.5703125" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.140625" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.85546875" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="16.85546875" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="15.85546875" collapsed="false"/>
+    <col min="10" max="11" bestFit="true" customWidth="true" width="37.5703125" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:11">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1519,13 +1555,31 @@
         <v>78</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1">
+        <v>83</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" s="29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1">
       <c r="A2" s="23">
         <v>1</v>
       </c>
@@ -1536,12 +1590,35 @@
         <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+      <c r="E2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2">
+        <v>123456</v>
+      </c>
+      <c r="I2">
+        <v>555000001</v>
+      </c>
+      <c r="J2" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" s="30" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="J2" r:id="rId2"/>
+    <hyperlink ref="K2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>